<commit_message>
Add los rebill a los missing records
</commit_message>
<xml_diff>
--- a/src/assets/files/cancel_missing_modelo.xlsx
+++ b/src/assets/files/cancel_missing_modelo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sites\clx-portalv2\src\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtanoira\eclipse-workspace\CLX-Documentacion\app-HotGoDatawarehouse\Documentacion\TablasModelo_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>userId</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>user</t>
+  </si>
+  <si>
+    <t>user_payment_id</t>
+  </si>
+  <si>
+    <t>UP_MX_hotgo_95345765_1605768224</t>
   </si>
 </sst>
 </file>
@@ -204,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -234,6 +240,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -515,11 +524,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,9 +539,10 @@
     <col min="5" max="5" width="21.88671875" style="7" customWidth="1"/>
     <col min="6" max="6" width="23" style="7" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" customWidth="1"/>
+    <col min="8" max="8" width="36.109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,8 +564,11 @@
       <c r="G1" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -574,8 +587,11 @@
       <c r="F2" s="7">
         <v>43301</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -583,7 +599,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
@@ -591,7 +607,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
@@ -599,7 +615,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
@@ -607,7 +623,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -615,7 +631,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>
     </row>
   </sheetData>

</xml_diff>